<commit_message>
Feat: seleciona e conta valores distintos na tabela songs.
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -954,7 +954,7 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -984,7 +984,7 @@
       </c>
       <c r="J9" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="4"/>
       <c r="B12" s="8"/>
       <c r="C12" s="4"/>
@@ -1060,7 +1060,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>61</v>
       </c>
@@ -1084,7 +1084,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4">
         <v>1</v>
       </c>
@@ -1108,7 +1108,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4">
         <v>2</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="4">
         <v>3</v>
       </c>
@@ -1156,7 +1156,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="4">
         <v>4</v>
       </c>
@@ -1180,7 +1180,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4">
         <v>5</v>
       </c>
@@ -1204,7 +1204,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4">
         <v>6</v>
       </c>

</xml_diff>